<commit_message>
Novas gráficos e tabelas
</commit_message>
<xml_diff>
--- a/ExcelPython2.xlsx
+++ b/ExcelPython2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T-Gamer\Documents\Desenvolvimento 2022\Python com Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FD2947-9004-464F-AAF4-3A7C6C853F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01C3B18-1015-466B-952C-3FD21FD6EC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{22A281B5-584D-42CE-BE44-50291AC267DA}"/>
   </bookViews>
@@ -60,7 +60,7 @@
     <t>Meta</t>
   </si>
   <si>
-    <t xml:space="preserve">Valor  </t>
+    <t xml:space="preserve">Marketcap </t>
   </si>
 </sst>
 </file>
@@ -160,16 +160,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mj-lt"/>
-              <a:ea typeface="+mj-ea"/>
-              <a:cs typeface="+mj-cs"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="pt-BR"/>
@@ -179,9 +179,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -192,21 +191,23 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Valor  </c:v>
+                  <c:v>Marketcap </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Planilha1!$A$2:$A$11</c:f>
@@ -222,10 +223,10 @@
                   <c:v>Microsoft</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>Saudi Aramco</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>Google</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Saudi Aramco</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Amazon</c:v>
@@ -237,10 +238,10 @@
                   <c:v>Tesla</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>Meta</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>Bitcoin</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Meta</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -252,41 +253,42 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>11882</c:v>
+                  <c:v>11384</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2695</c:v>
+                  <c:v>2614</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2488</c:v>
+                  <c:v>2254</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1775</c:v>
+                  <c:v>1965</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1844</c:v>
+                  <c:v>1729</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1775</c:v>
+                  <c:v>2821</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4400</c:v>
+                  <c:v>1227</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1135</c:v>
+                  <c:v>865</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1092</c:v>
+                  <c:v>826</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>908</c:v>
+                  <c:v>684</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8B5E-4F83-A52A-3FB94D1F205A}"/>
+              <c16:uniqueId val="{00000000-887F-4C26-8EAD-1A0706825C4F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -298,32 +300,17 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="267"/>
-        <c:overlap val="-43"/>
-        <c:axId val="491144368"/>
-        <c:axId val="491148960"/>
-      </c:barChart>
+        <c:smooth val="0"/>
+        <c:axId val="473211576"/>
+        <c:axId val="473206328"/>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="491144368"/>
+        <c:axId val="473211576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -332,7 +319,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="dk1">
+              <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
                 <a:lumOff val="85000"/>
               </a:schemeClr>
@@ -346,9 +333,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
+                  <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -361,7 +348,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="491148960"/>
+        <c:crossAx val="473206328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -369,7 +356,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="491148960"/>
+        <c:axId val="473206328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -379,7 +366,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="dk1">
+                <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -407,7 +394,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
+                  <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -420,28 +407,49 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="491144368"/>
+        <c:crossAx val="473211576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
-        <a:pattFill prst="ltDnDiag">
-          <a:fgClr>
-            <a:schemeClr val="dk1">
-              <a:lumMod val="15000"/>
-              <a:lumOff val="85000"/>
-            </a:schemeClr>
-          </a:fgClr>
-          <a:bgClr>
-            <a:schemeClr val="lt1"/>
-          </a:bgClr>
-        </a:pattFill>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -455,11 +463,11 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="dk1">
+        <a:schemeClr val="tx1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -527,25 +535,25 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="208">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -553,7 +561,7 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -561,22 +569,22 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="bg1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -584,14 +592,14 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="75000"/>
         <a:lumOff val="25000"/>
       </a:schemeClr>
@@ -628,12 +636,12 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -643,12 +651,12 @@
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -660,13 +668,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="22225" cap="rnd">
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -678,34 +686,33 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln w="15875">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -721,15 +728,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
+      <a:noFill/>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -737,7 +745,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="800" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
     <cs:lnRef idx="0"/>
@@ -749,18 +757,17 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -769,12 +776,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -788,14 +795,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -807,36 +814,29 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="ltDnDiag">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="lt1"/>
-        </a:bgClr>
-      </a:pattFill>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -847,12 +847,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
@@ -866,12 +866,31 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -879,18 +898,58 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -898,95 +957,18 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="ltDnDiag">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="lt1"/>
-        </a:bgClr>
-      </a:pattFill>
-    </cs:spPr>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="major">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -995,13 +977,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1010,7 +993,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -1028,14 +1011,13 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1044,7 +1026,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -1056,20 +1038,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="ltDnDiag">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="lt1"/>
-        </a:bgClr>
-      </a:pattFill>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
     </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
@@ -1080,22 +1055,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
+      <xdr:colOff>428625</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
+      <xdr:colOff>466725</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Gráfico 5">
+        <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C8266C7-685E-4AC6-BCCE-37FA36C4071E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{602CC2BD-CACC-4225-BA37-622E7805F8C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1416,12 +1391,13 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1438,7 +1414,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>11882</v>
+        <v>11384</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1446,7 +1422,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3">
-        <v>2695</v>
+        <v>2614</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1454,23 +1430,23 @@
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>2488</v>
+        <v>2254</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3">
-        <v>1775</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>1844</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1478,7 +1454,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3">
-        <v>1775</v>
+        <v>2821</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1486,7 +1462,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>4400</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1494,23 +1470,23 @@
         <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>1135</v>
+        <v>865</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="3">
-        <v>1092</v>
+        <v>826</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3">
-        <v>908</v>
+        <v>684</v>
       </c>
     </row>
   </sheetData>

</xml_diff>